<commit_message>
2024 data adding ticker name column
</commit_message>
<xml_diff>
--- a/data/Tickers_YTD_Returns_2024.xlsx
+++ b/data/Tickers_YTD_Returns_2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,25 +450,30 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Price Change YTD (%)</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Total Dividend</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Dividend Yield YTD (%)</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Unadjusted Total YTD (%)</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Adjusted Total YTD (%)</t>
         </is>
@@ -485,19 +490,24 @@
           <t>TLT</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>iShares 20+ Year Treasury Bond ETF</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
         <v>-11.68</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>3.76</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>3.8</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>-7.88</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>-8.050000000000001</v>
       </c>
     </row>
@@ -512,21 +522,26 @@
           <t>^GSPC</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>S&amp;P 500</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
         <v>23.31</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>23.31</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
         <v>23.31</v>
       </c>
+      <c r="H3" t="n">
+        <v>23.31</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -539,19 +554,24 @@
           <t>DIVO</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Amplify CWP Enhanced Dividend Income ETF</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
         <v>10.75</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>1.9</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>5.2</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>15.95</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>16.22</v>
       </c>
     </row>
@@ -566,19 +586,24 @@
           <t>FTHI</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>First Trust BuyWrite Income ETF</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
         <v>8.94</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>2</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>9.380000000000001</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>18.32</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>19.02</v>
       </c>
     </row>
@@ -593,19 +618,24 @@
           <t>SPYI</t>
         </is>
       </c>
-      <c r="C6" t="n">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Neos S&amp;P 500(R) High Income ETF</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
         <v>5.44</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>6.12</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>12.7</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>18.13</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>19.03</v>
       </c>
     </row>
@@ -620,19 +650,24 @@
           <t>RDVI</t>
         </is>
       </c>
-      <c r="C7" t="n">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>FT Vest Rising Dividend Achievers Target Income ETF</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
         <v>5.03</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>2.09</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>9.050000000000001</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>14.08</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>14.56</v>
       </c>
     </row>
@@ -647,19 +682,24 @@
           <t>JEPI</t>
         </is>
       </c>
-      <c r="C8" t="n">
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>JPMorgan Equity Premium Income ETF</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
         <v>4.64</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>4.22</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>7.67</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>12.31</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>12.57</v>
       </c>
     </row>
@@ -674,19 +714,24 @@
           <t>ISPY</t>
         </is>
       </c>
-      <c r="C9" t="n">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>ProShares S&amp;P 500 High Income ETF</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
         <v>9.630000000000001</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>4.36</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>10.78</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>20.41</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>21.31</v>
       </c>
     </row>
@@ -701,7 +746,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -722,25 +767,30 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Price Change YTD (%)</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Total Dividend</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Dividend Yield YTD (%)</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Unadjusted Total YTD (%)</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Adjusted Total YTD (%)</t>
         </is>
@@ -757,19 +807,24 @@
           <t>EMLP</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>First Trust North American Energy Infrastructure Fund</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
         <v>28.75</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>1.14</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>4.12</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>32.86</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>33.4</v>
       </c>
     </row>
@@ -784,19 +839,24 @@
           <t>MLPR</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>ETRACS Quarterly Pay 1.5X Leveraged Alerian MLP Index ETN</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
         <v>18.8</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>5.7</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>11.37</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>30.18</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>31.58</v>
       </c>
     </row>
@@ -811,19 +871,24 @@
           <t>AMLP</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Alerian MLP ETF</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
         <v>13.26</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>3.71</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>8.73</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>21.99</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>22.76</v>
       </c>
     </row>
@@ -838,7 +903,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -859,25 +924,30 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Price Change YTD (%)</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Total Dividend</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Dividend Yield YTD (%)</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Unadjusted Total YTD (%)</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Adjusted Total YTD (%)</t>
         </is>
@@ -894,19 +964,24 @@
           <t>ACWI</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>iShares MSCI ACWI ETF</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
         <v>15.46</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>2</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>1.97</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>17.42</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>17.45</v>
       </c>
     </row>
@@ -921,19 +996,24 @@
           <t>ACWV</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>iShares MSCI Global Min Vol Factor ETF</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
         <v>8.82</v>
-      </c>
-      <c r="D3" t="n">
-        <v>2.54</v>
       </c>
       <c r="E3" t="n">
         <v>2.54</v>
       </c>
       <c r="F3" t="n">
+        <v>2.54</v>
+      </c>
+      <c r="G3" t="n">
         <v>11.36</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>11.38</v>
       </c>
     </row>
@@ -948,19 +1028,24 @@
           <t>URTH</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>iShares MSCI World ETF</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
         <v>16.9</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>2.29</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>1.72</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>18.62</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>18.66</v>
       </c>
     </row>
@@ -975,19 +1060,24 @@
           <t>FLPSX</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Fidelity Low-Priced Stock</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
         <v>-7.53</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>6.62</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>15.01</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>7.48</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>7.23</v>
       </c>
     </row>
@@ -1002,19 +1092,24 @@
           <t>GVALX</t>
         </is>
       </c>
-      <c r="C6" t="n">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Gotham Large Value Institutional</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
         <v>1.1</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>1.48</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>10.84</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>11.94</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>11.72</v>
       </c>
     </row>
@@ -1029,19 +1124,24 @@
           <t>VMVFX</t>
         </is>
       </c>
-      <c r="C7" t="n">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Vanguard Global Minimum Volatility Inv</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
         <v>9.300000000000001</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>0.58</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>4.12</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>13.42</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>13.38</v>
       </c>
     </row>
@@ -1056,21 +1156,26 @@
           <t>^GSPC</t>
         </is>
       </c>
-      <c r="C8" t="n">
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>S&amp;P 500</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
         <v>23.31</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>23.31</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
         <v>23.31</v>
       </c>
+      <c r="H8" t="n">
+        <v>23.31</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1083,19 +1188,24 @@
           <t>CCGIX</t>
         </is>
       </c>
-      <c r="C9" t="n">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Baird Chautauqua Global Growth Instl</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
         <v>14.32</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>0.43</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>2.09</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>16.41</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>16.32</v>
       </c>
     </row>
@@ -1110,19 +1220,24 @@
           <t>SGENX</t>
         </is>
       </c>
-      <c r="C10" t="n">
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>First Eagle Global A</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
         <v>6.23</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>3.66</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>5.8</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>12.03</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>11.78</v>
       </c>
     </row>
@@ -1137,19 +1252,24 @@
           <t>WGNIX</t>
         </is>
       </c>
-      <c r="C11" t="n">
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Pabrai Wagons Institutional</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
         <v>9.93</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>0.15</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>1.36</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>11.29</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>11.17</v>
       </c>
     </row>
@@ -1164,21 +1284,26 @@
           <t>BRK-A</t>
         </is>
       </c>
-      <c r="C12" t="n">
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Berkshire Hathaway Inc.</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
         <v>25.49</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>25.49</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
         <v>25.49</v>
       </c>
+      <c r="H12" t="n">
+        <v>25.49</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1191,19 +1316,24 @@
           <t>MKL</t>
         </is>
       </c>
-      <c r="C13" t="n">
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Markel Group Inc.</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
         <v>21.57</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
       </c>
       <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
         <v>21.57</v>
       </c>
-      <c r="G13" t="n">
+      <c r="H13" t="n">
         <v>21.57</v>
       </c>
     </row>
@@ -1218,7 +1348,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1239,25 +1369,30 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Price Change YTD (%)</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Total Dividend</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Dividend Yield YTD (%)</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Unadjusted Total YTD (%)</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Adjusted Total YTD (%)</t>
         </is>
@@ -1274,21 +1409,26 @@
           <t>EWJV</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>iShares MSCI Japan Value ETF</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
         <v>7.2</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>1.28</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>4.39</v>
-      </c>
-      <c r="F2" t="n">
-        <v>11.59</v>
       </c>
       <c r="G2" t="n">
         <v>11.59</v>
       </c>
+      <c r="H2" t="n">
+        <v>11.59</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1301,19 +1441,24 @@
           <t>VWO</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Vanguard Emerging Markets Stock Index Fund</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
         <v>7.15</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>1.41</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>3.43</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>10.58</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>10.59</v>
       </c>
     </row>
@@ -1328,19 +1473,24 @@
           <t>HEDJ</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>WisdomTree Europe Hedged Equity Fund</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
         <v>2.03</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>1.43</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>3.35</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>5.38</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>5.28</v>
       </c>
     </row>
@@ -1355,19 +1505,24 @@
           <t>FNDE</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Schwab Fundamental Emerging Markets Equity ETF</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
         <v>7.04</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>1.4</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>5.16</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>12.2</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>12.09</v>
       </c>
     </row>
@@ -1382,19 +1537,24 @@
           <t>ADVE</t>
         </is>
       </c>
-      <c r="C6" t="n">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Matthews Asia Dividend Active ETF</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
         <v>1.02</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>1.92</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>6.06</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>7.08</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>7.02</v>
       </c>
     </row>
@@ -1409,19 +1569,24 @@
           <t>EEM</t>
         </is>
       </c>
-      <c r="C7" t="n">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>iShares MSCI Emerging Markets ETF</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
         <v>4</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>1.02</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>2.53</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>6.53</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>6.49</v>
       </c>
     </row>
@@ -1436,7 +1601,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1457,25 +1622,30 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Price Change YTD (%)</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Total Dividend</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Dividend Yield YTD (%)</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Unadjusted Total YTD (%)</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Adjusted Total YTD (%)</t>
         </is>
@@ -1492,21 +1662,26 @@
           <t>^GSPC</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>S&amp;P 500</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
         <v>23.31</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>23.31</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
         <v>23.31</v>
       </c>
+      <c r="H2" t="n">
+        <v>23.31</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1519,19 +1694,24 @@
           <t>GVLU</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Gotham 1000 Value ETF</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
         <v>8.140000000000001</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>0.68</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>3.12</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>11.25</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>11.1</v>
       </c>
     </row>
@@ -1546,19 +1726,24 @@
           <t>GSPY</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Gotham Enhanced 500 ETF</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
         <v>22.57</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>0.27</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>1.03</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>23.6</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>23.57</v>
       </c>
     </row>
@@ -1573,19 +1758,24 @@
           <t>RSP</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Invesco S&amp;P 500 Equal Weight ETF</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
         <v>11.05</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>2.66</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>1.68</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>12.73</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>12.79</v>
       </c>
     </row>
@@ -1600,19 +1790,24 @@
           <t>IWN</t>
         </is>
       </c>
-      <c r="C6" t="n">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>iShares Russell 2000 Value ETF</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
         <v>5.69</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>2.96</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>1.9</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>7.6</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>7.63</v>
       </c>
     </row>
@@ -1627,19 +1822,24 @@
           <t>GINDX</t>
         </is>
       </c>
-      <c r="C7" t="n">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Gotham Index Plus Institutional</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
         <v>22.23</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>0.82</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>3.63</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>25.86</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>25.79</v>
       </c>
     </row>
@@ -1654,19 +1854,24 @@
           <t>GSPFX</t>
         </is>
       </c>
-      <c r="C8" t="n">
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Gotham Enhanced S&amp;P 500 Index Instl</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
         <v>10.59</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>1.96</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>12.18</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>22.77</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>22.43</v>
       </c>
     </row>
@@ -1681,19 +1886,24 @@
           <t>SEQUX</t>
         </is>
       </c>
-      <c r="C9" t="n">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Sequoia</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
         <v>15.1</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>9.109999999999999</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>5.72</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>20.82</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>20.8</v>
       </c>
     </row>
@@ -1708,19 +1918,24 @@
           <t>FEVAX</t>
         </is>
       </c>
-      <c r="C10" t="n">
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>First Eagle US Value A</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
         <v>8.619999999999999</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>1.38</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>7.27</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>15.89</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>15.56</v>
       </c>
     </row>
@@ -1735,19 +1950,24 @@
           <t>FCNTX</t>
         </is>
       </c>
-      <c r="C11" t="n">
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Fidelity Contrafund</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
         <v>30.7</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>0.88</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>5.48</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>36.18</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>36</v>
       </c>
     </row>
@@ -1762,19 +1982,24 @@
           <t>FMAGX</t>
         </is>
       </c>
-      <c r="C12" t="n">
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Fidelity Magellan</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
         <v>20.47</v>
       </c>
-      <c r="D12" t="n">
+      <c r="E12" t="n">
         <v>0.91</v>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
         <v>7.37</v>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
         <v>27.84</v>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>28.06</v>
       </c>
     </row>
@@ -1789,19 +2014,24 @@
           <t>AKRIX</t>
         </is>
       </c>
-      <c r="C13" t="n">
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Akre Focus Instl</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
         <v>13.04</v>
       </c>
-      <c r="D13" t="n">
+      <c r="E13" t="n">
         <v>3.27</v>
       </c>
-      <c r="E13" t="n">
+      <c r="F13" t="n">
         <v>5.48</v>
       </c>
-      <c r="F13" t="n">
+      <c r="G13" t="n">
         <v>18.51</v>
       </c>
-      <c r="G13" t="n">
+      <c r="H13" t="n">
         <v>18.27</v>
       </c>
     </row>

</xml_diff>